<commit_message>
update Excel example with gender
</commit_message>
<xml_diff>
--- a/doc/Files/users_inscription_list.xlsx
+++ b/doc/Files/users_inscription_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>bo</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>gorgu@gadz.org</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SKF</t>
   </si>
 </sst>
 </file>
@@ -390,20 +399,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>701</v>
       </c>
@@ -421,7 +430,7 @@
       </c>
       <c r="F1" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>AxYy5546</v>
+        <v>IkMy5553</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -429,14 +438,17 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -454,7 +466,7 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(97,122))&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)&amp;RANDBETWEEN(0,9)</f>
-        <v>OkKh9207</v>
+        <v>GsAq9503</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -462,10 +474,16 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3">
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="3">
         <v>42069</v>
       </c>
     </row>
@@ -477,7 +495,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="I2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>